<commit_message>
updated master implan sectoring scheme
</commit_message>
<xml_diff>
--- a/data/interim/implan-import.xlsx
+++ b/data/interim/implan-import.xlsx
@@ -6,24 +6,24 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="bikeComm" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="bikeInd" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="campComm" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="campInd" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="fishComm" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="fishInd" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="huntComm" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="huntInd" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="picnicComm" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="picnicInd" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="snowComm" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="snowInd" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="trailComm" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="trailInd" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="waterComm" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="waterInd" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="wildlifeComm" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="wildlifeInd" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="bikeComm" sheetId="19" state="visible" r:id="rId1"/>
+    <sheet name="bikeInd" sheetId="20" state="visible" r:id="rId2"/>
+    <sheet name="campComm" sheetId="21" state="visible" r:id="rId3"/>
+    <sheet name="campInd" sheetId="22" state="visible" r:id="rId4"/>
+    <sheet name="fishComm" sheetId="23" state="visible" r:id="rId5"/>
+    <sheet name="fishInd" sheetId="24" state="visible" r:id="rId6"/>
+    <sheet name="huntComm" sheetId="25" state="visible" r:id="rId7"/>
+    <sheet name="huntInd" sheetId="26" state="visible" r:id="rId8"/>
+    <sheet name="picnicComm" sheetId="27" state="visible" r:id="rId9"/>
+    <sheet name="picnicInd" sheetId="28" state="visible" r:id="rId10"/>
+    <sheet name="snowComm" sheetId="29" state="visible" r:id="rId11"/>
+    <sheet name="snowInd" sheetId="30" state="visible" r:id="rId12"/>
+    <sheet name="trailComm" sheetId="31" state="visible" r:id="rId13"/>
+    <sheet name="trailInd" sheetId="32" state="visible" r:id="rId14"/>
+    <sheet name="waterComm" sheetId="33" state="visible" r:id="rId15"/>
+    <sheet name="waterInd" sheetId="34" state="visible" r:id="rId16"/>
+    <sheet name="wildlifeComm" sheetId="35" state="visible" r:id="rId17"/>
+    <sheet name="wildlifeInd" sheetId="36" state="visible" r:id="rId18"/>
   </sheets>
 </workbook>
 </file>
@@ -1770,7 +1770,7 @@
         <v>3393</v>
       </c>
       <c r="B79" t="n">
-        <v>718011.253373793</v>
+        <v>718011.253373792</v>
       </c>
       <c r="C79" t="n">
         <v>2019</v>
@@ -1804,7 +1804,7 @@
         <v>3395</v>
       </c>
       <c r="B81" t="n">
-        <v>631976.826108585</v>
+        <v>631976.826108586</v>
       </c>
       <c r="C81" t="n">
         <v>2019</v>
@@ -1821,7 +1821,7 @@
         <v>3396</v>
       </c>
       <c r="B82" t="n">
-        <v>918677.962864716</v>
+        <v>918677.962864717</v>
       </c>
       <c r="C82" t="n">
         <v>2019</v>
@@ -1855,7 +1855,7 @@
         <v>3398</v>
       </c>
       <c r="B84" t="n">
-        <v>665169.764964276</v>
+        <v>665169.764964278</v>
       </c>
       <c r="C84" t="n">
         <v>2019</v>
@@ -1872,7 +1872,7 @@
         <v>3399</v>
       </c>
       <c r="B85" t="n">
-        <v>97292.6332146306</v>
+        <v>97292.6332146308</v>
       </c>
       <c r="C85" t="n">
         <v>2019</v>
@@ -1889,7 +1889,7 @@
         <v>3400</v>
       </c>
       <c r="B86" t="n">
-        <v>906645.858360268</v>
+        <v>906645.858360269</v>
       </c>
       <c r="C86" t="n">
         <v>2019</v>
@@ -3857,7 +3857,7 @@
         <v>3392</v>
       </c>
       <c r="B78" t="n">
-        <v>637105.148970137</v>
+        <v>637105.148970136</v>
       </c>
       <c r="C78" t="n">
         <v>2019</v>
@@ -3891,7 +3891,7 @@
         <v>3394</v>
       </c>
       <c r="B80" t="n">
-        <v>767712.254247357</v>
+        <v>767712.254247356</v>
       </c>
       <c r="C80" t="n">
         <v>2019</v>
@@ -3942,7 +3942,7 @@
         <v>3397</v>
       </c>
       <c r="B83" t="n">
-        <v>539440.846406537</v>
+        <v>539440.846406536</v>
       </c>
       <c r="C83" t="n">
         <v>2019</v>
@@ -3959,7 +3959,7 @@
         <v>3398</v>
       </c>
       <c r="B84" t="n">
-        <v>1447888.73907524</v>
+        <v>1447888.73907525</v>
       </c>
       <c r="C84" t="n">
         <v>2019</v>
@@ -3976,7 +3976,7 @@
         <v>3399</v>
       </c>
       <c r="B85" t="n">
-        <v>211778.880289315</v>
+        <v>211778.880289316</v>
       </c>
       <c r="C85" t="n">
         <v>2019</v>
@@ -3993,7 +3993,7 @@
         <v>3400</v>
       </c>
       <c r="B86" t="n">
-        <v>1973514.72931055</v>
+        <v>1973514.72931056</v>
       </c>
       <c r="C86" t="n">
         <v>2019</v>
@@ -6247,7 +6247,7 @@
         <v>3392</v>
       </c>
       <c r="B78" t="n">
-        <v>1636645.64808038</v>
+        <v>1636645.64808037</v>
       </c>
       <c r="C78" t="n">
         <v>2019</v>
@@ -6264,7 +6264,7 @@
         <v>3393</v>
       </c>
       <c r="B79" t="n">
-        <v>4014925.45465557</v>
+        <v>4014925.45465556</v>
       </c>
       <c r="C79" t="n">
         <v>2019</v>
@@ -6298,7 +6298,7 @@
         <v>3395</v>
       </c>
       <c r="B81" t="n">
-        <v>3533844.12009329</v>
+        <v>3533844.1200933</v>
       </c>
       <c r="C81" t="n">
         <v>2019</v>
@@ -6315,7 +6315,7 @@
         <v>3396</v>
       </c>
       <c r="B82" t="n">
-        <v>5136999.62278515</v>
+        <v>5136999.62278516</v>
       </c>
       <c r="C82" t="n">
         <v>2019</v>
@@ -6349,7 +6349,7 @@
         <v>3398</v>
       </c>
       <c r="B84" t="n">
-        <v>3719450.09005594</v>
+        <v>3719450.09005595</v>
       </c>
       <c r="C84" t="n">
         <v>2019</v>
@@ -6366,7 +6366,7 @@
         <v>3399</v>
       </c>
       <c r="B85" t="n">
-        <v>544034.188612545</v>
+        <v>544034.188612546</v>
       </c>
       <c r="C85" t="n">
         <v>2019</v>
@@ -7285,7 +7285,7 @@
         <v>543</v>
       </c>
       <c r="B24" t="n">
-        <v>218521.931438371</v>
+        <v>218521.931438372</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
@@ -8773,7 +8773,7 @@
         <v>3393</v>
       </c>
       <c r="B86" t="n">
-        <v>2864260.98512895</v>
+        <v>2864260.98512894</v>
       </c>
       <c r="C86" t="n">
         <v>2019</v>
@@ -8807,7 +8807,7 @@
         <v>3395</v>
       </c>
       <c r="B88" t="n">
-        <v>2521055.98348622</v>
+        <v>2521055.98348623</v>
       </c>
       <c r="C88" t="n">
         <v>2019</v>
@@ -8824,7 +8824,7 @@
         <v>3396</v>
       </c>
       <c r="B89" t="n">
-        <v>3664752.37618774</v>
+        <v>3664752.37618775</v>
       </c>
       <c r="C89" t="n">
         <v>2019</v>
@@ -8858,7 +8858,7 @@
         <v>3398</v>
       </c>
       <c r="B91" t="n">
-        <v>2653467.89109825</v>
+        <v>2653467.89109826</v>
       </c>
       <c r="C91" t="n">
         <v>2019</v>
@@ -8875,7 +8875,7 @@
         <v>3399</v>
       </c>
       <c r="B92" t="n">
-        <v>388115.774157724</v>
+        <v>388115.774157725</v>
       </c>
       <c r="C92" t="n">
         <v>2019</v>
@@ -9794,7 +9794,7 @@
         <v>543</v>
       </c>
       <c r="B24" t="n">
-        <v>1069970.53210027</v>
+        <v>1069970.53210028</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
@@ -10993,13 +10993,13 @@
         <v>3182</v>
       </c>
       <c r="B69" t="n">
-        <v>19372.9713450709</v>
+        <v>19278.6169813287</v>
       </c>
       <c r="C69" t="n">
         <v>2019</v>
       </c>
       <c r="D69" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E69" t="n">
         <v>1</v>
@@ -11007,10 +11007,10 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>3183</v>
+        <v>3182</v>
       </c>
       <c r="B70" t="n">
-        <v>73226.9845953363</v>
+        <v>94.3543637422698</v>
       </c>
       <c r="C70" t="n">
         <v>2019</v>
@@ -11024,10 +11024,10 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>3184</v>
+        <v>3183</v>
       </c>
       <c r="B71" t="n">
-        <v>90651.6826705098</v>
+        <v>73226.9845953363</v>
       </c>
       <c r="C71" t="n">
         <v>2019</v>
@@ -11041,10 +11041,10 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>3185</v>
+        <v>3184</v>
       </c>
       <c r="B72" t="n">
-        <v>215133.759774843</v>
+        <v>90651.6826705098</v>
       </c>
       <c r="C72" t="n">
         <v>2019</v>
@@ -11058,10 +11058,10 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>3270</v>
+        <v>3185</v>
       </c>
       <c r="B73" t="n">
-        <v>9892150.88520613</v>
+        <v>215133.759774843</v>
       </c>
       <c r="C73" t="n">
         <v>2019</v>
@@ -11075,10 +11075,10 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>3271</v>
+        <v>3270</v>
       </c>
       <c r="B74" t="n">
-        <v>19268553.8584231</v>
+        <v>9892150.88520613</v>
       </c>
       <c r="C74" t="n">
         <v>2019</v>
@@ -11092,10 +11092,10 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>3340</v>
+        <v>3271</v>
       </c>
       <c r="B75" t="n">
-        <v>75915581.6380111</v>
+        <v>19268553.8584231</v>
       </c>
       <c r="C75" t="n">
         <v>2019</v>
@@ -11109,10 +11109,10 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>3341</v>
+        <v>3340</v>
       </c>
       <c r="B76" t="n">
-        <v>116398309.613734</v>
+        <v>75915581.6380111</v>
       </c>
       <c r="C76" t="n">
         <v>2019</v>
@@ -11126,10 +11126,10 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>3347</v>
+        <v>3341</v>
       </c>
       <c r="B77" t="n">
-        <v>416096.364944103</v>
+        <v>116398309.613734</v>
       </c>
       <c r="C77" t="n">
         <v>2019</v>
@@ -11143,10 +11143,10 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>3348</v>
+        <v>3347</v>
       </c>
       <c r="B78" t="n">
-        <v>276646.000450427</v>
+        <v>416096.364944103</v>
       </c>
       <c r="C78" t="n">
         <v>2019</v>
@@ -11160,10 +11160,10 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="B79" t="n">
-        <v>611345.690654174</v>
+        <v>276646.000450427</v>
       </c>
       <c r="C79" t="n">
         <v>2019</v>
@@ -11177,10 +11177,10 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>3350</v>
+        <v>3349</v>
       </c>
       <c r="B80" t="n">
-        <v>403650.242914814</v>
+        <v>611345.690654174</v>
       </c>
       <c r="C80" t="n">
         <v>2019</v>
@@ -11194,16 +11194,16 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>3351</v>
+        <v>3350</v>
       </c>
       <c r="B81" t="n">
-        <v>399350.326240718</v>
+        <v>403650.242914814</v>
       </c>
       <c r="C81" t="n">
         <v>2019</v>
       </c>
       <c r="D81" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E81" t="n">
         <v>1</v>
@@ -11211,16 +11211,16 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>3352</v>
+        <v>3351</v>
       </c>
       <c r="B82" t="n">
-        <v>910957.265284139</v>
+        <v>399350.326240718</v>
       </c>
       <c r="C82" t="n">
         <v>2019</v>
       </c>
       <c r="D82" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E82" t="n">
         <v>1</v>
@@ -11228,10 +11228,10 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>3353</v>
+        <v>3352</v>
       </c>
       <c r="B83" t="n">
-        <v>368552.191888983</v>
+        <v>910957.265284139</v>
       </c>
       <c r="C83" t="n">
         <v>2019</v>
@@ -11245,10 +11245,10 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>3361</v>
+        <v>3353</v>
       </c>
       <c r="B84" t="n">
-        <v>4840359.32397556</v>
+        <v>368552.191888983</v>
       </c>
       <c r="C84" t="n">
         <v>2019</v>
@@ -11262,10 +11262,10 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>3364</v>
+        <v>3361</v>
       </c>
       <c r="B85" t="n">
-        <v>25148656.2780529</v>
+        <v>4840359.32397556</v>
       </c>
       <c r="C85" t="n">
         <v>2019</v>
@@ -11279,10 +11279,10 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>3382</v>
+        <v>3364</v>
       </c>
       <c r="B86" t="n">
-        <v>9566479.63348978</v>
+        <v>25148656.2780529</v>
       </c>
       <c r="C86" t="n">
         <v>2019</v>
@@ -11296,10 +11296,10 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>3392</v>
+        <v>3382</v>
       </c>
       <c r="B87" t="n">
-        <v>54155.5969580514</v>
+        <v>9566479.63348978</v>
       </c>
       <c r="C87" t="n">
         <v>2019</v>
@@ -11313,10 +11313,10 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>3393</v>
+        <v>3392</v>
       </c>
       <c r="B88" t="n">
-        <v>132851.411662612</v>
+        <v>54155.5969580514</v>
       </c>
       <c r="C88" t="n">
         <v>2019</v>
@@ -11330,10 +11330,10 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>3394</v>
+        <v>3393</v>
       </c>
       <c r="B89" t="n">
-        <v>65257.5410636428</v>
+        <v>132851.411662612</v>
       </c>
       <c r="C89" t="n">
         <v>2019</v>
@@ -11347,10 +11347,10 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>3395</v>
+        <v>3394</v>
       </c>
       <c r="B90" t="n">
-        <v>116932.726460868</v>
+        <v>65257.5410636428</v>
       </c>
       <c r="C90" t="n">
         <v>2019</v>
@@ -11364,10 +11364,10 @@
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>3396</v>
+        <v>3395</v>
       </c>
       <c r="B91" t="n">
-        <v>169980.155124912</v>
+        <v>116932.726460868</v>
       </c>
       <c r="C91" t="n">
         <v>2019</v>
@@ -11381,10 +11381,10 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>3397</v>
+        <v>3396</v>
       </c>
       <c r="B92" t="n">
-        <v>45853.8768803325</v>
+        <v>169980.155124913</v>
       </c>
       <c r="C92" t="n">
         <v>2019</v>
@@ -11398,10 +11398,10 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>3398</v>
+        <v>3397</v>
       </c>
       <c r="B93" t="n">
-        <v>123074.31374587</v>
+        <v>45853.8768803324</v>
       </c>
       <c r="C93" t="n">
         <v>2019</v>
@@ -11415,10 +11415,10 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>3399</v>
+        <v>3398</v>
       </c>
       <c r="B94" t="n">
-        <v>18001.7563878034</v>
+        <v>123074.313745871</v>
       </c>
       <c r="C94" t="n">
         <v>2019</v>
@@ -11432,10 +11432,10 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>3400</v>
+        <v>3399</v>
       </c>
       <c r="B95" t="n">
-        <v>167753.891871827</v>
+        <v>18001.7563878034</v>
       </c>
       <c r="C95" t="n">
         <v>2019</v>
@@ -11449,10 +11449,10 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>3401</v>
+        <v>3400</v>
       </c>
       <c r="B96" t="n">
-        <v>189319.610098199</v>
+        <v>167753.891871827</v>
       </c>
       <c r="C96" t="n">
         <v>2019</v>
@@ -11466,10 +11466,10 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>3402</v>
+        <v>3401</v>
       </c>
       <c r="B97" t="n">
-        <v>41.0645770165527</v>
+        <v>189319.610098199</v>
       </c>
       <c r="C97" t="n">
         <v>2019</v>
@@ -11483,7 +11483,7 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>3403</v>
+        <v>3402</v>
       </c>
       <c r="B98" t="n">
         <v>41.0645770165527</v>
@@ -11500,10 +11500,10 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>3404</v>
+        <v>3403</v>
       </c>
       <c r="B99" t="n">
-        <v>51.3307212706908</v>
+        <v>41.0645770165527</v>
       </c>
       <c r="C99" t="n">
         <v>2019</v>
@@ -11517,10 +11517,10 @@
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>3405</v>
+        <v>3404</v>
       </c>
       <c r="B100" t="n">
-        <v>6703.79219795222</v>
+        <v>51.3307212706908</v>
       </c>
       <c r="C100" t="n">
         <v>2019</v>
@@ -11534,10 +11534,10 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>3406</v>
+        <v>3405</v>
       </c>
       <c r="B101" t="n">
-        <v>2100576.30812772</v>
+        <v>6703.79219795222</v>
       </c>
       <c r="C101" t="n">
         <v>2019</v>
@@ -11551,10 +11551,10 @@
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>3407</v>
+        <v>3406</v>
       </c>
       <c r="B102" t="n">
-        <v>41.0645770165527</v>
+        <v>2100576.30812772</v>
       </c>
       <c r="C102" t="n">
         <v>2019</v>
@@ -11568,10 +11568,10 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>3408</v>
+        <v>3407</v>
       </c>
       <c r="B103" t="n">
-        <v>665944.245477435</v>
+        <v>41.0645770165527</v>
       </c>
       <c r="C103" t="n">
         <v>2019</v>
@@ -11585,10 +11585,10 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>3409</v>
+        <v>3408</v>
       </c>
       <c r="B104" t="n">
-        <v>41.0645770165527</v>
+        <v>665944.245477435</v>
       </c>
       <c r="C104" t="n">
         <v>2019</v>
@@ -11602,7 +11602,7 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>3410</v>
+        <v>3409</v>
       </c>
       <c r="B105" t="n">
         <v>41.0645770165527</v>
@@ -11619,10 +11619,10 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>3411</v>
+        <v>3410</v>
       </c>
       <c r="B106" t="n">
-        <v>482.508779944494</v>
+        <v>41.0645770165527</v>
       </c>
       <c r="C106" t="n">
         <v>2019</v>
@@ -11636,10 +11636,10 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>3412</v>
+        <v>3411</v>
       </c>
       <c r="B107" t="n">
-        <v>7412.15615148776</v>
+        <v>482.508779944494</v>
       </c>
       <c r="C107" t="n">
         <v>2019</v>
@@ -11653,10 +11653,10 @@
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>3413</v>
+        <v>3412</v>
       </c>
       <c r="B108" t="n">
-        <v>41.0645770165527</v>
+        <v>7412.15615148776</v>
       </c>
       <c r="C108" t="n">
         <v>2019</v>
@@ -11670,16 +11670,16 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>3414</v>
+        <v>3413</v>
       </c>
       <c r="B109" t="n">
-        <v>17082.8640388859</v>
+        <v>41.0645770165527</v>
       </c>
       <c r="C109" t="n">
         <v>2019</v>
       </c>
       <c r="D109" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E109" t="n">
         <v>1</v>
@@ -11687,10 +11687,10 @@
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>3415</v>
+        <v>3414</v>
       </c>
       <c r="B110" t="n">
-        <v>741562.338819331</v>
+        <v>17082.8640388859</v>
       </c>
       <c r="C110" t="n">
         <v>2019</v>
@@ -11704,10 +11704,10 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>3416</v>
+        <v>3415</v>
       </c>
       <c r="B111" t="n">
-        <v>718740.700142382</v>
+        <v>741562.338819331</v>
       </c>
       <c r="C111" t="n">
         <v>2019</v>
@@ -11721,10 +11721,10 @@
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>3417</v>
+        <v>3416</v>
       </c>
       <c r="B112" t="n">
-        <v>210507.287931103</v>
+        <v>718740.700142382</v>
       </c>
       <c r="C112" t="n">
         <v>2019</v>
@@ -11738,10 +11738,10 @@
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>3418</v>
+        <v>3417</v>
       </c>
       <c r="B113" t="n">
-        <v>716851.72959962</v>
+        <v>210507.287931103</v>
       </c>
       <c r="C113" t="n">
         <v>2019</v>
@@ -11755,16 +11755,16 @@
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>3424</v>
+        <v>3418</v>
       </c>
       <c r="B114" t="n">
-        <v>1275628.47921416</v>
+        <v>716851.72959962</v>
       </c>
       <c r="C114" t="n">
         <v>2019</v>
       </c>
       <c r="D114" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E114" t="n">
         <v>1</v>
@@ -11772,10 +11772,10 @@
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>3426</v>
+        <v>3424</v>
       </c>
       <c r="B115" t="n">
-        <v>670492.327443684</v>
+        <v>1275628.47921416</v>
       </c>
       <c r="C115" t="n">
         <v>2019</v>
@@ -11789,10 +11789,10 @@
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>3427</v>
+        <v>3426</v>
       </c>
       <c r="B116" t="n">
-        <v>57673.53224418</v>
+        <v>670492.327443684</v>
       </c>
       <c r="C116" t="n">
         <v>2019</v>
@@ -11806,16 +11806,16 @@
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>3502</v>
+        <v>3427</v>
       </c>
       <c r="B117" t="n">
-        <v>114425.335372428</v>
+        <v>57673.53224418</v>
       </c>
       <c r="C117" t="n">
         <v>2019</v>
       </c>
       <c r="D117" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E117" t="n">
         <v>1</v>
@@ -11823,10 +11823,10 @@
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>3503</v>
+        <v>3502</v>
       </c>
       <c r="B118" t="n">
-        <v>177517.351435021</v>
+        <v>114425.335372428</v>
       </c>
       <c r="C118" t="n">
         <v>2019</v>
@@ -11840,10 +11840,10 @@
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>3524</v>
+        <v>3503</v>
       </c>
       <c r="B119" t="n">
-        <v>10876829.1530195</v>
+        <v>177517.351435021</v>
       </c>
       <c r="C119" t="n">
         <v>2019</v>
@@ -11857,10 +11857,10 @@
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>3525</v>
+        <v>3524</v>
       </c>
       <c r="B120" t="n">
-        <v>160911.114435237</v>
+        <v>10876829.1530195</v>
       </c>
       <c r="C120" t="n">
         <v>2019</v>
@@ -11874,18 +11874,35 @@
     </row>
     <row r="121">
       <c r="A121" t="n">
+        <v>3525</v>
+      </c>
+      <c r="B121" t="n">
+        <v>160911.114435237</v>
+      </c>
+      <c r="C121" t="n">
+        <v>2019</v>
+      </c>
+      <c r="D121" t="s">
+        <v>12</v>
+      </c>
+      <c r="E121" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
         <v>3536</v>
       </c>
-      <c r="B121" t="n">
+      <c r="B122" t="n">
         <v>-24033.0436989299</v>
       </c>
-      <c r="C121" t="n">
-        <v>2019</v>
-      </c>
-      <c r="D121" t="s">
-        <v>12</v>
-      </c>
-      <c r="E121" t="n">
+      <c r="C122" t="n">
+        <v>2019</v>
+      </c>
+      <c r="D122" t="s">
+        <v>12</v>
+      </c>
+      <c r="E122" t="n">
         <v>1</v>
       </c>
     </row>
@@ -13018,7 +13035,7 @@
         <v>543</v>
       </c>
       <c r="B24" t="n">
-        <v>60240.0918337494</v>
+        <v>60240.0918337496</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
@@ -14523,7 +14540,7 @@
         <v>3394</v>
       </c>
       <c r="B87" t="n">
-        <v>1880254.08392167</v>
+        <v>1880254.08392166</v>
       </c>
       <c r="C87" t="n">
         <v>2019</v>
@@ -14557,7 +14574,7 @@
         <v>3396</v>
       </c>
       <c r="B89" t="n">
-        <v>4897608.393604</v>
+        <v>4897608.39360401</v>
       </c>
       <c r="C89" t="n">
         <v>2019</v>
@@ -14591,7 +14608,7 @@
         <v>3398</v>
       </c>
       <c r="B91" t="n">
-        <v>3546118.61364565</v>
+        <v>3546118.61364566</v>
       </c>
       <c r="C91" t="n">
         <v>2019</v>
@@ -14608,7 +14625,7 @@
         <v>3399</v>
       </c>
       <c r="B92" t="n">
-        <v>518681.449135816</v>
+        <v>518681.449135817</v>
       </c>
       <c r="C92" t="n">
         <v>2019</v>
@@ -14625,7 +14642,7 @@
         <v>3400</v>
       </c>
       <c r="B93" t="n">
-        <v>4833463.46099894</v>
+        <v>4833463.46099895</v>
       </c>
       <c r="C93" t="n">
         <v>2019</v>
@@ -15527,7 +15544,7 @@
         <v>543</v>
       </c>
       <c r="B24" t="n">
-        <v>1047388.01315292</v>
+        <v>1047388.01315293</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
@@ -16998,7 +17015,7 @@
         <v>3393</v>
       </c>
       <c r="B85" t="n">
-        <v>474323.56965849</v>
+        <v>474323.569658489</v>
       </c>
       <c r="C85" t="n">
         <v>2019</v>
@@ -17032,7 +17049,7 @@
         <v>3395</v>
       </c>
       <c r="B87" t="n">
-        <v>417488.587668712</v>
+        <v>417488.587668713</v>
       </c>
       <c r="C87" t="n">
         <v>2019</v>
@@ -17049,7 +17066,7 @@
         <v>3396</v>
       </c>
       <c r="B88" t="n">
-        <v>606885.489141118</v>
+        <v>606885.489141119</v>
       </c>
       <c r="C88" t="n">
         <v>2019</v>
@@ -17083,7 +17100,7 @@
         <v>3398</v>
       </c>
       <c r="B90" t="n">
-        <v>439416.089739896</v>
+        <v>439416.089739898</v>
       </c>
       <c r="C90" t="n">
         <v>2019</v>
@@ -17100,7 +17117,7 @@
         <v>3399</v>
       </c>
       <c r="B91" t="n">
-        <v>64272.2365018605</v>
+        <v>64272.2365018607</v>
       </c>
       <c r="C91" t="n">
         <v>2019</v>
@@ -17117,7 +17134,7 @@
         <v>3400</v>
       </c>
       <c r="B92" t="n">
-        <v>598936.991492596</v>
+        <v>598936.991492597</v>
       </c>
       <c r="C92" t="n">
         <v>2019</v>
@@ -17134,7 +17151,7 @@
         <v>3401</v>
       </c>
       <c r="B93" t="n">
-        <v>675933.752937329</v>
+        <v>675933.752937328</v>
       </c>
       <c r="C93" t="n">
         <v>2019</v>
@@ -18095,7 +18112,7 @@
         <v>541</v>
       </c>
       <c r="B23" t="n">
-        <v>700216.193463541</v>
+        <v>700216.193463542</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
@@ -19405,13 +19422,13 @@
         <v>3256</v>
       </c>
       <c r="B74" t="n">
-        <v>6558875.24500846</v>
+        <v>5644995.65645779</v>
       </c>
       <c r="C74" t="n">
         <v>2019</v>
       </c>
       <c r="D74" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E74" t="n">
         <v>1</v>
@@ -19419,10 +19436,10 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>3257</v>
+        <v>3256</v>
       </c>
       <c r="B75" t="n">
-        <v>17230615.7488712</v>
+        <v>913879.588550669</v>
       </c>
       <c r="C75" t="n">
         <v>2019</v>
@@ -19436,10 +19453,10 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>3270</v>
+        <v>3257</v>
       </c>
       <c r="B76" t="n">
-        <v>2411131.41554226</v>
+        <v>17230615.7488712</v>
       </c>
       <c r="C76" t="n">
         <v>2019</v>
@@ -19453,10 +19470,10 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>3284</v>
+        <v>3270</v>
       </c>
       <c r="B77" t="n">
-        <v>1142.36750627794</v>
+        <v>2411131.41554226</v>
       </c>
       <c r="C77" t="n">
         <v>2019</v>
@@ -19470,10 +19487,10 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>3341</v>
+        <v>3284</v>
       </c>
       <c r="B78" t="n">
-        <v>19363456.8699324</v>
+        <v>1142.36750627794</v>
       </c>
       <c r="C78" t="n">
         <v>2019</v>
@@ -19487,10 +19504,10 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>3361</v>
+        <v>3341</v>
       </c>
       <c r="B79" t="n">
-        <v>9404.55403312553</v>
+        <v>19363456.8699324</v>
       </c>
       <c r="C79" t="n">
         <v>2019</v>
@@ -19504,10 +19521,10 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>3364</v>
+        <v>3361</v>
       </c>
       <c r="B80" t="n">
-        <v>5042749.02515966</v>
+        <v>9404.55403312553</v>
       </c>
       <c r="C80" t="n">
         <v>2019</v>
@@ -19521,10 +19538,10 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>3382</v>
+        <v>3364</v>
       </c>
       <c r="B81" t="n">
-        <v>17100983.5173776</v>
+        <v>5042749.02515966</v>
       </c>
       <c r="C81" t="n">
         <v>2019</v>
@@ -19538,10 +19555,10 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>3392</v>
+        <v>3382</v>
       </c>
       <c r="B82" t="n">
-        <v>39099.5792908444</v>
+        <v>17100983.5173776</v>
       </c>
       <c r="C82" t="n">
         <v>2019</v>
@@ -19555,10 +19572,10 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>3393</v>
+        <v>3392</v>
       </c>
       <c r="B83" t="n">
-        <v>95916.8506299815</v>
+        <v>39099.5792908443</v>
       </c>
       <c r="C83" t="n">
         <v>2019</v>
@@ -19572,10 +19589,10 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>3394</v>
+        <v>3393</v>
       </c>
       <c r="B84" t="n">
-        <v>47115.026783286</v>
+        <v>95916.8506299814</v>
       </c>
       <c r="C84" t="n">
         <v>2019</v>
@@ -19589,10 +19606,10 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>3395</v>
+        <v>3394</v>
       </c>
       <c r="B85" t="n">
-        <v>84423.7838148617</v>
+        <v>47115.026783286</v>
       </c>
       <c r="C85" t="n">
         <v>2019</v>
@@ -19606,10 +19623,10 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>3396</v>
+        <v>3395</v>
       </c>
       <c r="B86" t="n">
-        <v>122723.281184115</v>
+        <v>84423.7838148618</v>
       </c>
       <c r="C86" t="n">
         <v>2019</v>
@@ -19623,10 +19640,10 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>3397</v>
+        <v>3396</v>
       </c>
       <c r="B87" t="n">
-        <v>33105.8541606312</v>
+        <v>122723.281184115</v>
       </c>
       <c r="C87" t="n">
         <v>2019</v>
@@ -19640,10 +19657,10 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>3398</v>
+        <v>3397</v>
       </c>
       <c r="B88" t="n">
-        <v>88857.9234515756</v>
+        <v>33105.8541606312</v>
       </c>
       <c r="C88" t="n">
         <v>2019</v>
@@ -19657,10 +19674,10 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>3399</v>
+        <v>3398</v>
       </c>
       <c r="B89" t="n">
-        <v>12997.0149125046</v>
+        <v>88857.923451576</v>
       </c>
       <c r="C89" t="n">
         <v>2019</v>
@@ -19674,10 +19691,10 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>3400</v>
+        <v>3399</v>
       </c>
       <c r="B90" t="n">
-        <v>121115.950428371</v>
+        <v>12997.0149125046</v>
       </c>
       <c r="C90" t="n">
         <v>2019</v>
@@ -19691,10 +19708,10 @@
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>3401</v>
+        <v>3400</v>
       </c>
       <c r="B91" t="n">
-        <v>136686.095660252</v>
+        <v>121115.950428372</v>
       </c>
       <c r="C91" t="n">
         <v>2019</v>
@@ -19708,10 +19725,10 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>3402</v>
+        <v>3401</v>
       </c>
       <c r="B92" t="n">
-        <v>29.6480470217581</v>
+        <v>136686.095660252</v>
       </c>
       <c r="C92" t="n">
         <v>2019</v>
@@ -19725,7 +19742,7 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>3403</v>
+        <v>3402</v>
       </c>
       <c r="B93" t="n">
         <v>29.6480470217581</v>
@@ -19742,10 +19759,10 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>3404</v>
+        <v>3403</v>
       </c>
       <c r="B94" t="n">
-        <v>37.0600587771976</v>
+        <v>29.6480470217581</v>
       </c>
       <c r="C94" t="n">
         <v>2019</v>
@@ -19759,10 +19776,10 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>3405</v>
+        <v>3404</v>
       </c>
       <c r="B95" t="n">
-        <v>4840.043676302</v>
+        <v>37.0600587771976</v>
       </c>
       <c r="C95" t="n">
         <v>2019</v>
@@ -19776,10 +19793,10 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>3406</v>
+        <v>3405</v>
       </c>
       <c r="B96" t="n">
-        <v>1516586.54930399</v>
+        <v>4840.043676302</v>
       </c>
       <c r="C96" t="n">
         <v>2019</v>
@@ -19793,10 +19810,10 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>3407</v>
+        <v>3406</v>
       </c>
       <c r="B97" t="n">
-        <v>29.6480470217581</v>
+        <v>1516586.54930399</v>
       </c>
       <c r="C97" t="n">
         <v>2019</v>
@@ -19810,10 +19827,10 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>3408</v>
+        <v>3407</v>
       </c>
       <c r="B98" t="n">
-        <v>480802.378551851</v>
+        <v>29.6480470217581</v>
       </c>
       <c r="C98" t="n">
         <v>2019</v>
@@ -19827,10 +19844,10 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>3409</v>
+        <v>3408</v>
       </c>
       <c r="B99" t="n">
-        <v>29.6480470217581</v>
+        <v>480802.378551851</v>
       </c>
       <c r="C99" t="n">
         <v>2019</v>
@@ -19844,7 +19861,7 @@
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>3410</v>
+        <v>3409</v>
       </c>
       <c r="B100" t="n">
         <v>29.6480470217581</v>
@@ -19861,10 +19878,10 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>3411</v>
+        <v>3410</v>
       </c>
       <c r="B101" t="n">
-        <v>348.364552505657</v>
+        <v>29.6480470217581</v>
       </c>
       <c r="C101" t="n">
         <v>2019</v>
@@ -19878,10 +19895,10 @@
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>3412</v>
+        <v>3411</v>
       </c>
       <c r="B102" t="n">
-        <v>5351.47248742733</v>
+        <v>348.364552505657</v>
       </c>
       <c r="C102" t="n">
         <v>2019</v>
@@ -19895,10 +19912,10 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>3413</v>
+        <v>3412</v>
       </c>
       <c r="B103" t="n">
-        <v>29.6480470217581</v>
+        <v>5351.47248742733</v>
       </c>
       <c r="C103" t="n">
         <v>2019</v>
@@ -19912,16 +19929,16 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>3414</v>
+        <v>3413</v>
       </c>
       <c r="B104" t="n">
-        <v>12333.5875610514</v>
+        <v>29.6480470217581</v>
       </c>
       <c r="C104" t="n">
         <v>2019</v>
       </c>
       <c r="D104" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E104" t="n">
         <v>1</v>
@@ -19929,10 +19946,10 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>3415</v>
+        <v>3414</v>
       </c>
       <c r="B105" t="n">
-        <v>164092.871605501</v>
+        <v>12333.5875610514</v>
       </c>
       <c r="C105" t="n">
         <v>2019</v>
@@ -19946,10 +19963,10 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>3416</v>
+        <v>3415</v>
       </c>
       <c r="B106" t="n">
-        <v>147615.969473159</v>
+        <v>164092.871605501</v>
       </c>
       <c r="C106" t="n">
         <v>2019</v>
@@ -19963,10 +19980,10 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>3417</v>
+        <v>3416</v>
       </c>
       <c r="B107" t="n">
-        <v>151983.301045287</v>
+        <v>147615.969473159</v>
       </c>
       <c r="C107" t="n">
         <v>2019</v>
@@ -19980,10 +19997,10 @@
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>3418</v>
+        <v>3417</v>
       </c>
       <c r="B108" t="n">
-        <v>146252.159310158</v>
+        <v>151983.301045287</v>
       </c>
       <c r="C108" t="n">
         <v>2019</v>
@@ -19997,16 +20014,16 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>3424</v>
+        <v>3418</v>
       </c>
       <c r="B109" t="n">
-        <v>573356.20925266</v>
+        <v>146252.159310158</v>
       </c>
       <c r="C109" t="n">
         <v>2019</v>
       </c>
       <c r="D109" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E109" t="n">
         <v>1</v>
@@ -20014,7 +20031,7 @@
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>3425</v>
+        <v>3424</v>
       </c>
       <c r="B110" t="n">
         <v>573356.20925266</v>
@@ -20031,18 +20048,35 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
+        <v>3425</v>
+      </c>
+      <c r="B111" t="n">
+        <v>573356.20925266</v>
+      </c>
+      <c r="C111" t="n">
+        <v>2019</v>
+      </c>
+      <c r="D111" t="s">
+        <v>11</v>
+      </c>
+      <c r="E111" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
         <v>3536</v>
       </c>
-      <c r="B111" t="n">
+      <c r="B112" t="n">
         <v>-17351.5195194784</v>
       </c>
-      <c r="C111" t="n">
-        <v>2019</v>
-      </c>
-      <c r="D111" t="s">
-        <v>12</v>
-      </c>
-      <c r="E111" t="n">
+      <c r="C112" t="n">
+        <v>2019</v>
+      </c>
+      <c r="D112" t="s">
+        <v>12</v>
+      </c>
+      <c r="E112" t="n">
         <v>1</v>
       </c>
     </row>
@@ -21844,7 +21878,7 @@
         <v>3398</v>
       </c>
       <c r="B77" t="n">
-        <v>1532194.25969215</v>
+        <v>1532194.25969216</v>
       </c>
       <c r="C77" t="n">
         <v>2019</v>

</xml_diff>

<commit_message>
more implan margin error corrections
</commit_message>
<xml_diff>
--- a/data/interim/implan-import.xlsx
+++ b/data/interim/implan-import.xlsx
@@ -6,24 +6,24 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="bikeComm" sheetId="19" state="visible" r:id="rId1"/>
-    <sheet name="bikeInd" sheetId="20" state="visible" r:id="rId2"/>
-    <sheet name="campComm" sheetId="21" state="visible" r:id="rId3"/>
-    <sheet name="campInd" sheetId="22" state="visible" r:id="rId4"/>
-    <sheet name="fishComm" sheetId="23" state="visible" r:id="rId5"/>
-    <sheet name="fishInd" sheetId="24" state="visible" r:id="rId6"/>
-    <sheet name="huntComm" sheetId="25" state="visible" r:id="rId7"/>
-    <sheet name="huntInd" sheetId="26" state="visible" r:id="rId8"/>
-    <sheet name="picnicComm" sheetId="27" state="visible" r:id="rId9"/>
-    <sheet name="picnicInd" sheetId="28" state="visible" r:id="rId10"/>
-    <sheet name="snowComm" sheetId="29" state="visible" r:id="rId11"/>
-    <sheet name="snowInd" sheetId="30" state="visible" r:id="rId12"/>
-    <sheet name="trailComm" sheetId="31" state="visible" r:id="rId13"/>
-    <sheet name="trailInd" sheetId="32" state="visible" r:id="rId14"/>
-    <sheet name="waterComm" sheetId="33" state="visible" r:id="rId15"/>
-    <sheet name="waterInd" sheetId="34" state="visible" r:id="rId16"/>
-    <sheet name="wildlifeComm" sheetId="35" state="visible" r:id="rId17"/>
-    <sheet name="wildlifeInd" sheetId="36" state="visible" r:id="rId18"/>
+    <sheet name="bikeComm" sheetId="37" state="visible" r:id="rId1"/>
+    <sheet name="bikeInd" sheetId="38" state="visible" r:id="rId2"/>
+    <sheet name="campComm" sheetId="39" state="visible" r:id="rId3"/>
+    <sheet name="campInd" sheetId="40" state="visible" r:id="rId4"/>
+    <sheet name="fishComm" sheetId="41" state="visible" r:id="rId5"/>
+    <sheet name="fishInd" sheetId="42" state="visible" r:id="rId6"/>
+    <sheet name="huntComm" sheetId="43" state="visible" r:id="rId7"/>
+    <sheet name="huntInd" sheetId="44" state="visible" r:id="rId8"/>
+    <sheet name="picnicComm" sheetId="45" state="visible" r:id="rId9"/>
+    <sheet name="picnicInd" sheetId="46" state="visible" r:id="rId10"/>
+    <sheet name="snowComm" sheetId="47" state="visible" r:id="rId11"/>
+    <sheet name="snowInd" sheetId="48" state="visible" r:id="rId12"/>
+    <sheet name="trailComm" sheetId="49" state="visible" r:id="rId13"/>
+    <sheet name="trailInd" sheetId="50" state="visible" r:id="rId14"/>
+    <sheet name="waterComm" sheetId="51" state="visible" r:id="rId15"/>
+    <sheet name="waterInd" sheetId="52" state="visible" r:id="rId16"/>
+    <sheet name="wildlifeComm" sheetId="53" state="visible" r:id="rId17"/>
+    <sheet name="wildlifeInd" sheetId="54" state="visible" r:id="rId18"/>
   </sheets>
 </workbook>
 </file>
@@ -1623,7 +1623,7 @@
         <v>2019</v>
       </c>
       <c r="D70" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E70" t="n">
         <v>1</v>
@@ -3727,7 +3727,7 @@
         <v>2019</v>
       </c>
       <c r="D70" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E70" t="n">
         <v>1</v>
@@ -6117,7 +6117,7 @@
         <v>2019</v>
       </c>
       <c r="D70" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E70" t="n">
         <v>1</v>
@@ -8507,7 +8507,7 @@
         <v>2019</v>
       </c>
       <c r="D70" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E70" t="n">
         <v>1</v>
@@ -10993,7 +10993,7 @@
         <v>3182</v>
       </c>
       <c r="B69" t="n">
-        <v>19278.6169813287</v>
+        <v>19372.9713450709</v>
       </c>
       <c r="C69" t="n">
         <v>2019</v>
@@ -11007,10 +11007,10 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>3182</v>
+        <v>3183</v>
       </c>
       <c r="B70" t="n">
-        <v>94.3543637422698</v>
+        <v>73226.9845953363</v>
       </c>
       <c r="C70" t="n">
         <v>2019</v>
@@ -11024,10 +11024,10 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>3183</v>
+        <v>3184</v>
       </c>
       <c r="B71" t="n">
-        <v>73226.9845953363</v>
+        <v>90651.6826705098</v>
       </c>
       <c r="C71" t="n">
         <v>2019</v>
@@ -11041,10 +11041,10 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>3184</v>
+        <v>3185</v>
       </c>
       <c r="B72" t="n">
-        <v>90651.6826705098</v>
+        <v>215133.759774843</v>
       </c>
       <c r="C72" t="n">
         <v>2019</v>
@@ -11058,10 +11058,10 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>3185</v>
+        <v>3270</v>
       </c>
       <c r="B73" t="n">
-        <v>215133.759774843</v>
+        <v>9892150.88520613</v>
       </c>
       <c r="C73" t="n">
         <v>2019</v>
@@ -11075,10 +11075,10 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>3270</v>
+        <v>3271</v>
       </c>
       <c r="B74" t="n">
-        <v>9892150.88520613</v>
+        <v>19268553.8584231</v>
       </c>
       <c r="C74" t="n">
         <v>2019</v>
@@ -11092,10 +11092,10 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>3271</v>
+        <v>3340</v>
       </c>
       <c r="B75" t="n">
-        <v>19268553.8584231</v>
+        <v>75915581.6380111</v>
       </c>
       <c r="C75" t="n">
         <v>2019</v>
@@ -11109,10 +11109,10 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>3340</v>
+        <v>3341</v>
       </c>
       <c r="B76" t="n">
-        <v>75915581.6380111</v>
+        <v>116398309.613734</v>
       </c>
       <c r="C76" t="n">
         <v>2019</v>
@@ -11126,10 +11126,10 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>3341</v>
+        <v>3347</v>
       </c>
       <c r="B77" t="n">
-        <v>116398309.613734</v>
+        <v>416096.364944103</v>
       </c>
       <c r="C77" t="n">
         <v>2019</v>
@@ -11143,10 +11143,10 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>3347</v>
+        <v>3348</v>
       </c>
       <c r="B78" t="n">
-        <v>416096.364944103</v>
+        <v>276646.000450427</v>
       </c>
       <c r="C78" t="n">
         <v>2019</v>
@@ -11160,10 +11160,10 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>3348</v>
+        <v>3349</v>
       </c>
       <c r="B79" t="n">
-        <v>276646.000450427</v>
+        <v>611345.690654174</v>
       </c>
       <c r="C79" t="n">
         <v>2019</v>
@@ -11177,10 +11177,10 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>3349</v>
+        <v>3350</v>
       </c>
       <c r="B80" t="n">
-        <v>611345.690654174</v>
+        <v>403650.242914814</v>
       </c>
       <c r="C80" t="n">
         <v>2019</v>
@@ -11194,16 +11194,16 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>3350</v>
+        <v>3351</v>
       </c>
       <c r="B81" t="n">
-        <v>403650.242914814</v>
+        <v>399350.326240718</v>
       </c>
       <c r="C81" t="n">
         <v>2019</v>
       </c>
       <c r="D81" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E81" t="n">
         <v>1</v>
@@ -11211,16 +11211,16 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>3351</v>
+        <v>3352</v>
       </c>
       <c r="B82" t="n">
-        <v>399350.326240718</v>
+        <v>910957.265284139</v>
       </c>
       <c r="C82" t="n">
         <v>2019</v>
       </c>
       <c r="D82" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E82" t="n">
         <v>1</v>
@@ -11228,10 +11228,10 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>3352</v>
+        <v>3353</v>
       </c>
       <c r="B83" t="n">
-        <v>910957.265284139</v>
+        <v>368552.191888983</v>
       </c>
       <c r="C83" t="n">
         <v>2019</v>
@@ -11245,10 +11245,10 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>3353</v>
+        <v>3361</v>
       </c>
       <c r="B84" t="n">
-        <v>368552.191888983</v>
+        <v>4840359.32397556</v>
       </c>
       <c r="C84" t="n">
         <v>2019</v>
@@ -11262,10 +11262,10 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>3361</v>
+        <v>3364</v>
       </c>
       <c r="B85" t="n">
-        <v>4840359.32397556</v>
+        <v>25148656.2780529</v>
       </c>
       <c r="C85" t="n">
         <v>2019</v>
@@ -11279,10 +11279,10 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>3364</v>
+        <v>3382</v>
       </c>
       <c r="B86" t="n">
-        <v>25148656.2780529</v>
+        <v>9566479.63348978</v>
       </c>
       <c r="C86" t="n">
         <v>2019</v>
@@ -11296,10 +11296,10 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>3382</v>
+        <v>3392</v>
       </c>
       <c r="B87" t="n">
-        <v>9566479.63348978</v>
+        <v>54155.5969580514</v>
       </c>
       <c r="C87" t="n">
         <v>2019</v>
@@ -11313,10 +11313,10 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>3392</v>
+        <v>3393</v>
       </c>
       <c r="B88" t="n">
-        <v>54155.5969580514</v>
+        <v>132851.411662612</v>
       </c>
       <c r="C88" t="n">
         <v>2019</v>
@@ -11330,10 +11330,10 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>3393</v>
+        <v>3394</v>
       </c>
       <c r="B89" t="n">
-        <v>132851.411662612</v>
+        <v>65257.5410636428</v>
       </c>
       <c r="C89" t="n">
         <v>2019</v>
@@ -11347,10 +11347,10 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>3394</v>
+        <v>3395</v>
       </c>
       <c r="B90" t="n">
-        <v>65257.5410636428</v>
+        <v>116932.726460868</v>
       </c>
       <c r="C90" t="n">
         <v>2019</v>
@@ -11364,10 +11364,10 @@
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>3395</v>
+        <v>3396</v>
       </c>
       <c r="B91" t="n">
-        <v>116932.726460868</v>
+        <v>169980.155124913</v>
       </c>
       <c r="C91" t="n">
         <v>2019</v>
@@ -11381,10 +11381,10 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>3396</v>
+        <v>3397</v>
       </c>
       <c r="B92" t="n">
-        <v>169980.155124913</v>
+        <v>45853.8768803324</v>
       </c>
       <c r="C92" t="n">
         <v>2019</v>
@@ -11398,10 +11398,10 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>3397</v>
+        <v>3398</v>
       </c>
       <c r="B93" t="n">
-        <v>45853.8768803324</v>
+        <v>123074.313745871</v>
       </c>
       <c r="C93" t="n">
         <v>2019</v>
@@ -11415,10 +11415,10 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>3398</v>
+        <v>3399</v>
       </c>
       <c r="B94" t="n">
-        <v>123074.313745871</v>
+        <v>18001.7563878034</v>
       </c>
       <c r="C94" t="n">
         <v>2019</v>
@@ -11432,10 +11432,10 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>3399</v>
+        <v>3400</v>
       </c>
       <c r="B95" t="n">
-        <v>18001.7563878034</v>
+        <v>167753.891871827</v>
       </c>
       <c r="C95" t="n">
         <v>2019</v>
@@ -11449,10 +11449,10 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>3400</v>
+        <v>3401</v>
       </c>
       <c r="B96" t="n">
-        <v>167753.891871827</v>
+        <v>189319.610098199</v>
       </c>
       <c r="C96" t="n">
         <v>2019</v>
@@ -11466,10 +11466,10 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>3401</v>
+        <v>3402</v>
       </c>
       <c r="B97" t="n">
-        <v>189319.610098199</v>
+        <v>41.0645770165527</v>
       </c>
       <c r="C97" t="n">
         <v>2019</v>
@@ -11483,7 +11483,7 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>3402</v>
+        <v>3403</v>
       </c>
       <c r="B98" t="n">
         <v>41.0645770165527</v>
@@ -11500,10 +11500,10 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>3403</v>
+        <v>3404</v>
       </c>
       <c r="B99" t="n">
-        <v>41.0645770165527</v>
+        <v>51.3307212706908</v>
       </c>
       <c r="C99" t="n">
         <v>2019</v>
@@ -11517,10 +11517,10 @@
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>3404</v>
+        <v>3405</v>
       </c>
       <c r="B100" t="n">
-        <v>51.3307212706908</v>
+        <v>6703.79219795222</v>
       </c>
       <c r="C100" t="n">
         <v>2019</v>
@@ -11534,10 +11534,10 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>3405</v>
+        <v>3406</v>
       </c>
       <c r="B101" t="n">
-        <v>6703.79219795222</v>
+        <v>2100576.30812772</v>
       </c>
       <c r="C101" t="n">
         <v>2019</v>
@@ -11551,10 +11551,10 @@
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>3406</v>
+        <v>3407</v>
       </c>
       <c r="B102" t="n">
-        <v>2100576.30812772</v>
+        <v>41.0645770165527</v>
       </c>
       <c r="C102" t="n">
         <v>2019</v>
@@ -11568,10 +11568,10 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>3407</v>
+        <v>3408</v>
       </c>
       <c r="B103" t="n">
-        <v>41.0645770165527</v>
+        <v>665944.245477435</v>
       </c>
       <c r="C103" t="n">
         <v>2019</v>
@@ -11585,10 +11585,10 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>3408</v>
+        <v>3409</v>
       </c>
       <c r="B104" t="n">
-        <v>665944.245477435</v>
+        <v>41.0645770165527</v>
       </c>
       <c r="C104" t="n">
         <v>2019</v>
@@ -11602,7 +11602,7 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>3409</v>
+        <v>3410</v>
       </c>
       <c r="B105" t="n">
         <v>41.0645770165527</v>
@@ -11619,10 +11619,10 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>3410</v>
+        <v>3411</v>
       </c>
       <c r="B106" t="n">
-        <v>41.0645770165527</v>
+        <v>482.508779944494</v>
       </c>
       <c r="C106" t="n">
         <v>2019</v>
@@ -11636,10 +11636,10 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>3411</v>
+        <v>3412</v>
       </c>
       <c r="B107" t="n">
-        <v>482.508779944494</v>
+        <v>7412.15615148776</v>
       </c>
       <c r="C107" t="n">
         <v>2019</v>
@@ -11653,10 +11653,10 @@
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>3412</v>
+        <v>3413</v>
       </c>
       <c r="B108" t="n">
-        <v>7412.15615148776</v>
+        <v>41.0645770165527</v>
       </c>
       <c r="C108" t="n">
         <v>2019</v>
@@ -11670,16 +11670,16 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>3413</v>
+        <v>3414</v>
       </c>
       <c r="B109" t="n">
-        <v>41.0645770165527</v>
+        <v>17082.8640388859</v>
       </c>
       <c r="C109" t="n">
         <v>2019</v>
       </c>
       <c r="D109" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E109" t="n">
         <v>1</v>
@@ -11687,10 +11687,10 @@
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>3414</v>
+        <v>3415</v>
       </c>
       <c r="B110" t="n">
-        <v>17082.8640388859</v>
+        <v>741562.338819331</v>
       </c>
       <c r="C110" t="n">
         <v>2019</v>
@@ -11704,10 +11704,10 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>3415</v>
+        <v>3416</v>
       </c>
       <c r="B111" t="n">
-        <v>741562.338819331</v>
+        <v>718740.700142382</v>
       </c>
       <c r="C111" t="n">
         <v>2019</v>
@@ -11721,10 +11721,10 @@
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>3416</v>
+        <v>3417</v>
       </c>
       <c r="B112" t="n">
-        <v>718740.700142382</v>
+        <v>210507.287931103</v>
       </c>
       <c r="C112" t="n">
         <v>2019</v>
@@ -11738,10 +11738,10 @@
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>3417</v>
+        <v>3418</v>
       </c>
       <c r="B113" t="n">
-        <v>210507.287931103</v>
+        <v>716851.72959962</v>
       </c>
       <c r="C113" t="n">
         <v>2019</v>
@@ -11755,16 +11755,16 @@
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>3418</v>
+        <v>3424</v>
       </c>
       <c r="B114" t="n">
-        <v>716851.72959962</v>
+        <v>1275628.47921416</v>
       </c>
       <c r="C114" t="n">
         <v>2019</v>
       </c>
       <c r="D114" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E114" t="n">
         <v>1</v>
@@ -11772,10 +11772,10 @@
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>3424</v>
+        <v>3426</v>
       </c>
       <c r="B115" t="n">
-        <v>1275628.47921416</v>
+        <v>670492.327443684</v>
       </c>
       <c r="C115" t="n">
         <v>2019</v>
@@ -11789,10 +11789,10 @@
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>3426</v>
+        <v>3427</v>
       </c>
       <c r="B116" t="n">
-        <v>670492.327443684</v>
+        <v>57673.53224418</v>
       </c>
       <c r="C116" t="n">
         <v>2019</v>
@@ -11806,16 +11806,16 @@
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>3427</v>
+        <v>3502</v>
       </c>
       <c r="B117" t="n">
-        <v>57673.53224418</v>
+        <v>114425.335372428</v>
       </c>
       <c r="C117" t="n">
         <v>2019</v>
       </c>
       <c r="D117" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E117" t="n">
         <v>1</v>
@@ -11823,10 +11823,10 @@
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>3502</v>
+        <v>3503</v>
       </c>
       <c r="B118" t="n">
-        <v>114425.335372428</v>
+        <v>177517.351435021</v>
       </c>
       <c r="C118" t="n">
         <v>2019</v>
@@ -11840,10 +11840,10 @@
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>3503</v>
+        <v>3524</v>
       </c>
       <c r="B119" t="n">
-        <v>177517.351435021</v>
+        <v>10876829.1530195</v>
       </c>
       <c r="C119" t="n">
         <v>2019</v>
@@ -11857,10 +11857,10 @@
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>3524</v>
+        <v>3525</v>
       </c>
       <c r="B120" t="n">
-        <v>10876829.1530195</v>
+        <v>160911.114435237</v>
       </c>
       <c r="C120" t="n">
         <v>2019</v>
@@ -11874,10 +11874,10 @@
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>3525</v>
+        <v>3536</v>
       </c>
       <c r="B121" t="n">
-        <v>160911.114435237</v>
+        <v>-24033.0436989299</v>
       </c>
       <c r="C121" t="n">
         <v>2019</v>
@@ -11886,23 +11886,6 @@
         <v>12</v>
       </c>
       <c r="E121" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="n">
-        <v>3536</v>
-      </c>
-      <c r="B122" t="n">
-        <v>-24033.0436989299</v>
-      </c>
-      <c r="C122" t="n">
-        <v>2019</v>
-      </c>
-      <c r="D122" t="s">
-        <v>12</v>
-      </c>
-      <c r="E122" t="n">
         <v>1</v>
       </c>
     </row>
@@ -14257,7 +14240,7 @@
         <v>2019</v>
       </c>
       <c r="D70" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E70" t="n">
         <v>1</v>
@@ -16800,7 +16783,7 @@
         <v>2019</v>
       </c>
       <c r="D72" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E72" t="n">
         <v>1</v>
@@ -19343,7 +19326,7 @@
         <v>2019</v>
       </c>
       <c r="D69" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E69" t="n">
         <v>1</v>
@@ -19422,7 +19405,7 @@
         <v>3256</v>
       </c>
       <c r="B74" t="n">
-        <v>5644995.65645779</v>
+        <v>6558875.24500846</v>
       </c>
       <c r="C74" t="n">
         <v>2019</v>
@@ -19436,10 +19419,10 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>3256</v>
+        <v>3257</v>
       </c>
       <c r="B75" t="n">
-        <v>913879.588550669</v>
+        <v>17230615.7488712</v>
       </c>
       <c r="C75" t="n">
         <v>2019</v>
@@ -19453,10 +19436,10 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>3257</v>
+        <v>3270</v>
       </c>
       <c r="B76" t="n">
-        <v>17230615.7488712</v>
+        <v>2411131.41554226</v>
       </c>
       <c r="C76" t="n">
         <v>2019</v>
@@ -19470,10 +19453,10 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>3270</v>
+        <v>3284</v>
       </c>
       <c r="B77" t="n">
-        <v>2411131.41554226</v>
+        <v>1142.36750627794</v>
       </c>
       <c r="C77" t="n">
         <v>2019</v>
@@ -19487,10 +19470,10 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>3284</v>
+        <v>3341</v>
       </c>
       <c r="B78" t="n">
-        <v>1142.36750627794</v>
+        <v>19363456.8699324</v>
       </c>
       <c r="C78" t="n">
         <v>2019</v>
@@ -19504,10 +19487,10 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>3341</v>
+        <v>3361</v>
       </c>
       <c r="B79" t="n">
-        <v>19363456.8699324</v>
+        <v>9404.55403312553</v>
       </c>
       <c r="C79" t="n">
         <v>2019</v>
@@ -19521,10 +19504,10 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>3361</v>
+        <v>3364</v>
       </c>
       <c r="B80" t="n">
-        <v>9404.55403312553</v>
+        <v>5042749.02515966</v>
       </c>
       <c r="C80" t="n">
         <v>2019</v>
@@ -19538,10 +19521,10 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>3364</v>
+        <v>3382</v>
       </c>
       <c r="B81" t="n">
-        <v>5042749.02515966</v>
+        <v>17100983.5173776</v>
       </c>
       <c r="C81" t="n">
         <v>2019</v>
@@ -19555,10 +19538,10 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>3382</v>
+        <v>3392</v>
       </c>
       <c r="B82" t="n">
-        <v>17100983.5173776</v>
+        <v>39099.5792908443</v>
       </c>
       <c r="C82" t="n">
         <v>2019</v>
@@ -19572,10 +19555,10 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>3392</v>
+        <v>3393</v>
       </c>
       <c r="B83" t="n">
-        <v>39099.5792908443</v>
+        <v>95916.8506299814</v>
       </c>
       <c r="C83" t="n">
         <v>2019</v>
@@ -19589,10 +19572,10 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>3393</v>
+        <v>3394</v>
       </c>
       <c r="B84" t="n">
-        <v>95916.8506299814</v>
+        <v>47115.026783286</v>
       </c>
       <c r="C84" t="n">
         <v>2019</v>
@@ -19606,10 +19589,10 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>3394</v>
+        <v>3395</v>
       </c>
       <c r="B85" t="n">
-        <v>47115.026783286</v>
+        <v>84423.7838148618</v>
       </c>
       <c r="C85" t="n">
         <v>2019</v>
@@ -19623,10 +19606,10 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>3395</v>
+        <v>3396</v>
       </c>
       <c r="B86" t="n">
-        <v>84423.7838148618</v>
+        <v>122723.281184115</v>
       </c>
       <c r="C86" t="n">
         <v>2019</v>
@@ -19640,10 +19623,10 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>3396</v>
+        <v>3397</v>
       </c>
       <c r="B87" t="n">
-        <v>122723.281184115</v>
+        <v>33105.8541606312</v>
       </c>
       <c r="C87" t="n">
         <v>2019</v>
@@ -19657,10 +19640,10 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>3397</v>
+        <v>3398</v>
       </c>
       <c r="B88" t="n">
-        <v>33105.8541606312</v>
+        <v>88857.923451576</v>
       </c>
       <c r="C88" t="n">
         <v>2019</v>
@@ -19674,10 +19657,10 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>3398</v>
+        <v>3399</v>
       </c>
       <c r="B89" t="n">
-        <v>88857.923451576</v>
+        <v>12997.0149125046</v>
       </c>
       <c r="C89" t="n">
         <v>2019</v>
@@ -19691,10 +19674,10 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>3399</v>
+        <v>3400</v>
       </c>
       <c r="B90" t="n">
-        <v>12997.0149125046</v>
+        <v>121115.950428372</v>
       </c>
       <c r="C90" t="n">
         <v>2019</v>
@@ -19708,10 +19691,10 @@
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>3400</v>
+        <v>3401</v>
       </c>
       <c r="B91" t="n">
-        <v>121115.950428372</v>
+        <v>136686.095660252</v>
       </c>
       <c r="C91" t="n">
         <v>2019</v>
@@ -19725,10 +19708,10 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>3401</v>
+        <v>3402</v>
       </c>
       <c r="B92" t="n">
-        <v>136686.095660252</v>
+        <v>29.6480470217581</v>
       </c>
       <c r="C92" t="n">
         <v>2019</v>
@@ -19742,7 +19725,7 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>3402</v>
+        <v>3403</v>
       </c>
       <c r="B93" t="n">
         <v>29.6480470217581</v>
@@ -19759,10 +19742,10 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>3403</v>
+        <v>3404</v>
       </c>
       <c r="B94" t="n">
-        <v>29.6480470217581</v>
+        <v>37.0600587771976</v>
       </c>
       <c r="C94" t="n">
         <v>2019</v>
@@ -19776,10 +19759,10 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>3404</v>
+        <v>3405</v>
       </c>
       <c r="B95" t="n">
-        <v>37.0600587771976</v>
+        <v>4840.043676302</v>
       </c>
       <c r="C95" t="n">
         <v>2019</v>
@@ -19793,10 +19776,10 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>3405</v>
+        <v>3406</v>
       </c>
       <c r="B96" t="n">
-        <v>4840.043676302</v>
+        <v>1516586.54930399</v>
       </c>
       <c r="C96" t="n">
         <v>2019</v>
@@ -19810,10 +19793,10 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>3406</v>
+        <v>3407</v>
       </c>
       <c r="B97" t="n">
-        <v>1516586.54930399</v>
+        <v>29.6480470217581</v>
       </c>
       <c r="C97" t="n">
         <v>2019</v>
@@ -19827,10 +19810,10 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>3407</v>
+        <v>3408</v>
       </c>
       <c r="B98" t="n">
-        <v>29.6480470217581</v>
+        <v>480802.378551851</v>
       </c>
       <c r="C98" t="n">
         <v>2019</v>
@@ -19844,10 +19827,10 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>3408</v>
+        <v>3409</v>
       </c>
       <c r="B99" t="n">
-        <v>480802.378551851</v>
+        <v>29.6480470217581</v>
       </c>
       <c r="C99" t="n">
         <v>2019</v>
@@ -19861,7 +19844,7 @@
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>3409</v>
+        <v>3410</v>
       </c>
       <c r="B100" t="n">
         <v>29.6480470217581</v>
@@ -19878,10 +19861,10 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>3410</v>
+        <v>3411</v>
       </c>
       <c r="B101" t="n">
-        <v>29.6480470217581</v>
+        <v>348.364552505657</v>
       </c>
       <c r="C101" t="n">
         <v>2019</v>
@@ -19895,10 +19878,10 @@
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>3411</v>
+        <v>3412</v>
       </c>
       <c r="B102" t="n">
-        <v>348.364552505657</v>
+        <v>5351.47248742733</v>
       </c>
       <c r="C102" t="n">
         <v>2019</v>
@@ -19912,10 +19895,10 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>3412</v>
+        <v>3413</v>
       </c>
       <c r="B103" t="n">
-        <v>5351.47248742733</v>
+        <v>29.6480470217581</v>
       </c>
       <c r="C103" t="n">
         <v>2019</v>
@@ -19929,16 +19912,16 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>3413</v>
+        <v>3414</v>
       </c>
       <c r="B104" t="n">
-        <v>29.6480470217581</v>
+        <v>12333.5875610514</v>
       </c>
       <c r="C104" t="n">
         <v>2019</v>
       </c>
       <c r="D104" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E104" t="n">
         <v>1</v>
@@ -19946,10 +19929,10 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>3414</v>
+        <v>3415</v>
       </c>
       <c r="B105" t="n">
-        <v>12333.5875610514</v>
+        <v>164092.871605501</v>
       </c>
       <c r="C105" t="n">
         <v>2019</v>
@@ -19963,10 +19946,10 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>3415</v>
+        <v>3416</v>
       </c>
       <c r="B106" t="n">
-        <v>164092.871605501</v>
+        <v>147615.969473159</v>
       </c>
       <c r="C106" t="n">
         <v>2019</v>
@@ -19980,10 +19963,10 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>3416</v>
+        <v>3417</v>
       </c>
       <c r="B107" t="n">
-        <v>147615.969473159</v>
+        <v>151983.301045287</v>
       </c>
       <c r="C107" t="n">
         <v>2019</v>
@@ -19997,10 +19980,10 @@
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>3417</v>
+        <v>3418</v>
       </c>
       <c r="B108" t="n">
-        <v>151983.301045287</v>
+        <v>146252.159310158</v>
       </c>
       <c r="C108" t="n">
         <v>2019</v>
@@ -20014,16 +19997,16 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>3418</v>
+        <v>3424</v>
       </c>
       <c r="B109" t="n">
-        <v>146252.159310158</v>
+        <v>573356.20925266</v>
       </c>
       <c r="C109" t="n">
         <v>2019</v>
       </c>
       <c r="D109" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E109" t="n">
         <v>1</v>
@@ -20031,7 +20014,7 @@
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>3424</v>
+        <v>3425</v>
       </c>
       <c r="B110" t="n">
         <v>573356.20925266</v>
@@ -20048,35 +20031,18 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>3425</v>
+        <v>3536</v>
       </c>
       <c r="B111" t="n">
-        <v>573356.20925266</v>
+        <v>-17351.5195194784</v>
       </c>
       <c r="C111" t="n">
         <v>2019</v>
       </c>
       <c r="D111" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E111" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="n">
-        <v>3536</v>
-      </c>
-      <c r="B112" t="n">
-        <v>-17351.5195194784</v>
-      </c>
-      <c r="C112" t="n">
-        <v>2019</v>
-      </c>
-      <c r="D112" t="s">
-        <v>12</v>
-      </c>
-      <c r="E112" t="n">
         <v>1</v>
       </c>
     </row>
@@ -21714,7 +21680,7 @@
         <v>2019</v>
       </c>
       <c r="D67" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E67" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
update for new implan package version
</commit_message>
<xml_diff>
--- a/data/interim/implan-import.xlsx
+++ b/data/interim/implan-import.xlsx
@@ -6,24 +6,24 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="bikeComm" sheetId="55" state="visible" r:id="rId1"/>
-    <sheet name="bikeInd" sheetId="56" state="visible" r:id="rId2"/>
-    <sheet name="campComm" sheetId="57" state="visible" r:id="rId3"/>
-    <sheet name="campInd" sheetId="58" state="visible" r:id="rId4"/>
-    <sheet name="fishComm" sheetId="59" state="visible" r:id="rId5"/>
-    <sheet name="fishInd" sheetId="60" state="visible" r:id="rId6"/>
-    <sheet name="huntComm" sheetId="61" state="visible" r:id="rId7"/>
-    <sheet name="huntInd" sheetId="62" state="visible" r:id="rId8"/>
-    <sheet name="picnicComm" sheetId="63" state="visible" r:id="rId9"/>
-    <sheet name="picnicInd" sheetId="64" state="visible" r:id="rId10"/>
-    <sheet name="snowComm" sheetId="65" state="visible" r:id="rId11"/>
-    <sheet name="snowInd" sheetId="66" state="visible" r:id="rId12"/>
-    <sheet name="trailComm" sheetId="67" state="visible" r:id="rId13"/>
-    <sheet name="trailInd" sheetId="68" state="visible" r:id="rId14"/>
-    <sheet name="waterComm" sheetId="69" state="visible" r:id="rId15"/>
-    <sheet name="waterInd" sheetId="70" state="visible" r:id="rId16"/>
-    <sheet name="wildlifeComm" sheetId="71" state="visible" r:id="rId17"/>
-    <sheet name="wildlifeInd" sheetId="72" state="visible" r:id="rId18"/>
+    <sheet name="bikeComm" sheetId="73" state="visible" r:id="rId1"/>
+    <sheet name="bikeInd" sheetId="74" state="visible" r:id="rId2"/>
+    <sheet name="campComm" sheetId="75" state="visible" r:id="rId3"/>
+    <sheet name="campInd" sheetId="76" state="visible" r:id="rId4"/>
+    <sheet name="fishComm" sheetId="77" state="visible" r:id="rId5"/>
+    <sheet name="fishInd" sheetId="78" state="visible" r:id="rId6"/>
+    <sheet name="huntComm" sheetId="79" state="visible" r:id="rId7"/>
+    <sheet name="huntInd" sheetId="80" state="visible" r:id="rId8"/>
+    <sheet name="picnicComm" sheetId="81" state="visible" r:id="rId9"/>
+    <sheet name="picnicInd" sheetId="82" state="visible" r:id="rId10"/>
+    <sheet name="snowComm" sheetId="83" state="visible" r:id="rId11"/>
+    <sheet name="snowInd" sheetId="84" state="visible" r:id="rId12"/>
+    <sheet name="trailComm" sheetId="85" state="visible" r:id="rId13"/>
+    <sheet name="trailInd" sheetId="86" state="visible" r:id="rId14"/>
+    <sheet name="waterComm" sheetId="87" state="visible" r:id="rId15"/>
+    <sheet name="waterInd" sheetId="88" state="visible" r:id="rId16"/>
+    <sheet name="wildlifeComm" sheetId="89" state="visible" r:id="rId17"/>
+    <sheet name="wildlifeInd" sheetId="90" state="visible" r:id="rId18"/>
   </sheets>
 </workbook>
 </file>

</xml_diff>